<commit_message>
update to ESSR row in mapping file - wrong age data source for males+jacks listed
</commit_message>
<xml_diff>
--- a/termNIT/2023/R_OUT - TERMNIT_mapping_2023-output_from_02.xlsx
+++ b/termNIT/2023/R_OUT - TERMNIT_mapping_2023-output_from_02.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DAVIDSONKA\Documents\ANALYSIS\WCVI_Chinook_Term_Run_Recon\WCVI_CN_TermRunRecon\termNIT\2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53BD0587-F32F-4286-AB3C-B4523D45B0C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86B7510-5EA6-4F07-9110-C069D4EB56F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -623,8 +623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>